<commit_message>
I have collected a bunch of data and began doing analysis on the articles collected in order to fine tune the data collection. I had to remove (Review) from the list of reference keywords because everything was failing. I believe I am able to successfully collect all the data that I intended except for corresponding authors. The next phase is dispaying the info in a table in the UI. The following phase is export to excel and the last phase is the reflection
</commit_message>
<xml_diff>
--- a/example_output.xlsx
+++ b/example_output.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9465" xr2:uid="{CE12F41E-FF6A-46F6-AC6E-C903C98125B0}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="6825" windowHeight="2775" xr2:uid="{CE12F41E-FF6A-46F6-AC6E-C903C98125B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB3476C-923A-45C0-8E1A-18915BD22BA7}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>